<commit_message>
generate trainer und segler
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung.xlsx
+++ b/Zeitaufzeichnung.xlsx
@@ -371,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E14"/>
+  <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,23 +382,32 @@
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1">
         <v>42068</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>42069</v>
+      </c>
+      <c r="E2" s="1">
+        <v>42071</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -406,7 +415,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -414,32 +423,54 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>225</v>
+      </c>
+      <c r="E6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C13">
         <f>C3+C4+C5+C6</f>
         <v>220</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:E13" si="0">D3+D4+D5+D6</f>
-        <v>0</v>
+        <f t="shared" ref="D13:F13" si="0">D3+D4+D5+D6</f>
+        <v>240</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C14">
         <f>C13/60</f>
         <v>3.6666666666666665</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:F14" si="1">D13/60</f>
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generate boot, tourenboot, sportboot und mannschaft
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung.xlsx
+++ b/Zeitaufzeichnung.xlsx
@@ -374,7 +374,7 @@
   <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
         <v>225</v>
       </c>
       <c r="E6">
-        <v>60</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -448,7 +448,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>360</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
@@ -466,7 +466,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
generate bildet, zugewiesen, nimmt_teil
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung.xlsx
+++ b/Zeitaufzeichnung.xlsx
@@ -374,7 +374,7 @@
   <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,6 +395,9 @@
       <c r="E2" s="1">
         <v>42071</v>
       </c>
+      <c r="F2" s="1">
+        <v>42072</v>
+      </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -435,6 +438,9 @@
       </c>
       <c r="E6">
         <v>360</v>
+      </c>
+      <c r="F6">
+        <v>390</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -452,7 +458,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -470,7 +476,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Protokollierung + sql anfragen fertig
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung.xlsx
+++ b/Zeitaufzeichnung.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Datenbank &amp; User erstellen</t>
   </si>
@@ -32,6 +32,15 @@
   </si>
   <si>
     <t>Aufgabe                                       Datum</t>
+  </si>
+  <si>
+    <t>Generator Kommentieren</t>
+  </si>
+  <si>
+    <t>Java und JDBC</t>
+  </si>
+  <si>
+    <t>Java und JDBC Kommentieren</t>
   </si>
 </sst>
 </file>
@@ -374,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R14"/>
+  <dimension ref="B2:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,6 +454,9 @@
       <c r="D3">
         <v>15</v>
       </c>
+      <c r="O3">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -484,6 +496,9 @@
       <c r="H6">
         <v>10</v>
       </c>
+      <c r="N6">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -495,137 +510,170 @@
       <c r="H7">
         <v>170</v>
       </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <f>C3+C4+C5+C6+C7+C8+C9+C10</f>
-        <v>220</v>
-      </c>
-      <c r="D13">
-        <f t="shared" ref="D13:Q13" si="0">D3+D4+D5+D6+D7+D8+D9+D10</f>
-        <v>240</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>450</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13+Q13</f>
-        <v>1535</v>
+      <c r="J7">
+        <v>15</v>
+      </c>
+      <c r="O7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="O10">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C14">
-        <f>C13/60</f>
+        <f t="shared" ref="C14:Q14" si="0">C3+C4+C5+C6+C7+C9+C10+C11</f>
+        <v>220</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14+Q14</f>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>C14/60</f>
         <v>3.6666666666666665</v>
       </c>
-      <c r="D14">
-        <f t="shared" ref="D14:R14" si="1">D13/60</f>
+      <c r="D15">
+        <f t="shared" ref="D15:R15" si="1">D14/60</f>
         <v>4</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <f t="shared" si="1"/>
         <v>1.4166666666666667</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="1"/>
-        <v>25.583333333333332</v>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>28.333333333333332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>